<commit_message>
added od data from oa chemostat batch experiment
</commit_message>
<xml_diff>
--- a/data/251208_at_chemostat_d_03/plate_reader/251208_t0_absorbance.xlsx
+++ b/data/251208_at_chemostat_d_03/plate_reader/251208_t0_absorbance.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -237,64 +237,68 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -492,678 +496,678 @@
   </sheetPr>
   <dimension ref="A3:O44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29:H29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="31.71"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="H14" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="I14" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J14" s="2" t="n">
+      <c r="J14" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="K14" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="L14" s="2" t="n">
+      <c r="L14" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="M14" s="2" t="n">
+      <c r="M14" s="3" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="4" t="n">
         <v>0.271</v>
       </c>
-      <c r="C15" s="4" t="n">
+      <c r="C15" s="5" t="n">
         <v>0.294</v>
       </c>
-      <c r="D15" s="4" t="n">
+      <c r="D15" s="5" t="n">
         <v>0.311</v>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="E15" s="5" t="n">
         <v>0.279</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="5" t="n">
         <v>0.284</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="5" t="n">
         <v>0.303</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="5" t="n">
         <v>0.308</v>
       </c>
-      <c r="I15" s="4" t="n">
+      <c r="I15" s="5" t="n">
         <v>0.319</v>
       </c>
-      <c r="J15" s="4" t="n">
+      <c r="J15" s="5" t="n">
         <v>0.321</v>
       </c>
-      <c r="K15" s="4" t="n">
+      <c r="K15" s="5" t="n">
         <v>0.086</v>
       </c>
-      <c r="L15" s="4" t="n">
+      <c r="L15" s="5" t="n">
         <v>0.085</v>
       </c>
-      <c r="M15" s="5" t="n">
+      <c r="M15" s="6" t="n">
         <v>0.085</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="8"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="10" t="n">
         <v>0.09</v>
       </c>
-      <c r="C22" s="10" t="n">
+      <c r="C22" s="11" t="n">
         <v>0.094</v>
       </c>
-      <c r="D22" s="10" t="n">
+      <c r="D22" s="11" t="n">
         <v>0.1</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O24" s="12"/>
+      <c r="O24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="C25" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H25" s="2" t="n">
+      <c r="H25" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I25" s="2" t="n">
+      <c r="I25" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J25" s="2" t="n">
+      <c r="J25" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="K25" s="2" t="n">
+      <c r="K25" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="L25" s="2" t="n">
+      <c r="L25" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="M25" s="2" t="n">
+      <c r="M25" s="3" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="4" t="n">
         <v>0.177</v>
       </c>
-      <c r="C26" s="4" t="n">
+      <c r="C26" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="D26" s="4" t="n">
+      <c r="D26" s="5" t="n">
         <v>0.217</v>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="5" t="n">
         <v>0.184</v>
       </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="5" t="n">
         <v>0.19</v>
       </c>
-      <c r="G26" s="4" t="n">
+      <c r="G26" s="5" t="n">
         <v>0.209</v>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="5" t="n">
         <v>0.214</v>
       </c>
-      <c r="I26" s="4" t="n">
+      <c r="I26" s="5" t="n">
         <v>0.225</v>
       </c>
-      <c r="J26" s="4" t="n">
+      <c r="J26" s="5" t="n">
         <v>0.226</v>
       </c>
-      <c r="K26" s="4" t="n">
-        <v>-0.008</v>
-      </c>
-      <c r="L26" s="4" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="M26" s="5" t="n">
-        <v>-0.009</v>
+      <c r="K26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="8"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="14" t="n">
+      <c r="B29" s="15" t="n">
         <f aca="false">AVERAGE(B26:D26)</f>
         <v>0.198</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7" t="n">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8" t="n">
         <f aca="false">AVERAGE(E26:G26)</f>
         <v>0.194333333333333</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7" t="n">
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8" t="n">
         <f aca="false">AVERAGE(H26:J26)</f>
         <v>0.221666666666667</v>
       </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="8"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="8"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="8"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="11"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="12"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="2" t="n">
+      <c r="B36" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C36" s="2" t="n">
+      <c r="C36" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D36" s="2" t="n">
+      <c r="D36" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E36" s="2" t="n">
+      <c r="E36" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="F36" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G36" s="2" t="n">
+      <c r="G36" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H36" s="2" t="n">
+      <c r="H36" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I36" s="2" t="n">
+      <c r="I36" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="J36" s="2" t="n">
+      <c r="J36" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="K36" s="2" t="n">
+      <c r="K36" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="L36" s="2" t="n">
+      <c r="L36" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="M36" s="2" t="n">
+      <c r="M36" s="3" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="3" t="n">
+      <c r="B37" s="4" t="n">
         <v>0.177</v>
       </c>
-      <c r="C37" s="4" t="n">
+      <c r="C37" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="D37" s="4" t="n">
+      <c r="D37" s="5" t="n">
         <v>0.217</v>
       </c>
-      <c r="E37" s="4" t="n">
+      <c r="E37" s="5" t="n">
         <v>0.184</v>
       </c>
-      <c r="F37" s="4" t="n">
+      <c r="F37" s="5" t="n">
         <v>0.19</v>
       </c>
-      <c r="G37" s="4" t="n">
+      <c r="G37" s="5" t="n">
         <v>0.209</v>
       </c>
-      <c r="H37" s="4" t="n">
+      <c r="H37" s="5" t="n">
         <v>0.214</v>
       </c>
-      <c r="I37" s="4" t="n">
+      <c r="I37" s="5" t="n">
         <v>0.225</v>
       </c>
-      <c r="J37" s="4" t="n">
+      <c r="J37" s="5" t="n">
         <v>0.226</v>
       </c>
-      <c r="K37" s="4" t="n">
+      <c r="K37" s="5" t="n">
         <v>-0.008</v>
       </c>
-      <c r="L37" s="4" t="n">
+      <c r="L37" s="5" t="n">
         <v>-0.01</v>
       </c>
-      <c r="M37" s="5" t="n">
+      <c r="M37" s="6" t="n">
         <v>-0.009</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="8"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="8"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="8"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="8"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="8"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="11"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>